<commit_message>
Aggiunto telegramma per il fine curva
- Aggiornato excel telegrammi
- Aggiunto telegramma valore #8 per il reset delle variabili cinematiche
</commit_message>
<xml_diff>
--- a/gitsim_app/docs/Telegrammi.xlsx
+++ b/gitsim_app/docs/Telegrammi.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wasab\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Xilinx\Vivado\Projects\gitsim_python\gitsim_python.sdk\gitsim_app\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{541B4EA0-0261-468C-AB71-384DACEADB06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C290DC03-9A0F-4CD4-A280-49885C3F9DB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C33ADFD0-58CE-44BB-8514-68000BF8319E}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="74">
   <si>
     <t>0o00</t>
   </si>
@@ -253,6 +253,12 @@
   </si>
   <si>
     <t>0x07</t>
+  </si>
+  <si>
+    <t>Fine curva/reset</t>
+  </si>
+  <si>
+    <t>0x08</t>
   </si>
 </sst>
 </file>
@@ -1157,7 +1163,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1296,10 +1302,18 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="A10" s="19"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="4"/>
+      <c r="A10" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="11" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A11" s="9"/>

</xml_diff>